<commit_message>
Minor changes to handle Omega csv files. Needs more work.
</commit_message>
<xml_diff>
--- a/CureReportBuilder/Sample Files/Cure Report_Template - Complete.xlsx
+++ b/CureReportBuilder/Sample Files/Cure Report_Template - Complete.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will.Eagan\source\repos\CureReportBuilder\CureReportBuilder\Sample Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F0BDF8-9435-40A8-81B8-90CCD8013CF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2325" yWindow="1200" windowWidth="25035" windowHeight="13605"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cure Report" sheetId="14" r:id="rId1"/>
@@ -20,14 +26,6 @@
     <definedName name="PONum">'Cure Report'!$B$4</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -747,6 +745,42 @@
     <r>
       <rPr>
         <b/>
+        <u/>
+        <sz val="14"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+      </rPr>
+      <t>Part</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="14"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+48777-100
+Rev. C
+ARRW SHROUD COMPOSITE
+Qty: 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Palatino Linotype"/>
@@ -798,7 +832,6 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
         <rFont val="Palatino Linotype"/>
         <family val="1"/>
       </rPr>
@@ -994,25 +1027,18 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">RAMP UP
+</t>
+    </r>
+    <r>
       <rPr>
-        <b/>
         <u/>
-        <sz val="14"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Palatino Linotype"/>
         <family val="1"/>
       </rPr>
-      <t>Part</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="14"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+      <t>(FAIL)</t>
     </r>
     <r>
       <rPr>
@@ -1022,25 +1048,6 @@
         <family val="1"/>
       </rPr>
       <t xml:space="preserve">
-48777-100
-Rev. C
-ARRW SHROUD COMPOSITE
-Qty: 1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">RAMP UP
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">(PASS)
 </t>
     </r>
     <r>
@@ -1058,7 +1065,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="h:mm:ss\ AM/PM;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]dd\-mmm\-yyyy;@"/>
@@ -1067,7 +1074,7 @@
     <numFmt numFmtId="168" formatCode="h:mm\ AM/PM;@"/>
     <numFmt numFmtId="169" formatCode="[$-F0000]dd\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1310,6 +1317,19 @@
       <b/>
       <sz val="24"/>
       <color rgb="FF00B050"/>
+      <name val="Palatino Linotype"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Palatino Linotype"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Palatino Linotype"/>
       <family val="1"/>
     </font>
@@ -1795,6 +1815,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1806,12 +1832,6 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1831,6 +1851,12 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1842,12 +1868,6 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1911,7 +1931,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3981,7 +4001,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-9E00-404D-955F-255EB74B7098}"/>
             </c:ext>
@@ -6026,7 +6046,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-9E00-404D-955F-255EB74B7098}"/>
             </c:ext>
@@ -6059,6 +6079,11 @@
             </c:numLit>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B410-4C26-8988-19BFA3BB8EAF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -6079,6 +6104,11 @@
             </c:numLit>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B410-4C26-8988-19BFA3BB8EAF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -6099,6 +6129,11 @@
             </c:numLit>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B410-4C26-8988-19BFA3BB8EAF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -6136,7 +6171,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -6173,7 +6207,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -6188,7 +6221,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -6203,14 +6235,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:txPr>
     <a:bodyPr/>
@@ -6236,7 +6268,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -8293,7 +8325,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-AF2A-4E73-BD83-E5831FC93BEE}"/>
             </c:ext>
@@ -10328,7 +10360,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-AF2A-4E73-BD83-E5831FC93BEE}"/>
             </c:ext>
@@ -10431,14 +10463,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -10468,7 +10500,7 @@
         <xdr:cNvPr id="5" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10511,7 +10543,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{39749C52-B2EB-4B2D-A302-99560FCBC8E0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39749C52-B2EB-4B2D-A302-99560FCBC8E0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10821,19 +10853,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:T46"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:L4"/>
+      <selection activeCell="A40" sqref="A40:B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10845,22 +10877,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
       <c r="K2" s="36"/>
       <c r="L2" s="36"/>
       <c r="M2" s="36"/>
@@ -10873,82 +10905,82 @@
       <c r="T2" s="36"/>
     </row>
     <row r="3" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
+      <c r="A3" s="49"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
     </row>
     <row r="4" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="54" t="s">
+      <c r="A4" s="49"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="54"/>
-      <c r="M4" s="53" t="s">
+      <c r="L4" s="38"/>
+      <c r="M4" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="N4" s="53"/>
-      <c r="O4" s="53"/>
-      <c r="P4" s="53"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
       <c r="Q4" s="27" t="s">
         <v>4</v>
       </c>
       <c r="R4" s="28"/>
     </row>
     <row r="5" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41" t="s">
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
       <c r="L5" s="27"/>
       <c r="Q5" s="27"/>
     </row>
     <row r="6" spans="1:20" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="42"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
+      <c r="A6" s="50"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="55" t="s">
         <v>58</v>
       </c>
       <c r="E6" s="55"/>
       <c r="F6" s="55"/>
       <c r="G6" s="55"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="54" t="s">
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="54"/>
-      <c r="M6" s="53"/>
-      <c r="N6" s="53"/>
-      <c r="O6" s="53"/>
-      <c r="P6" s="53"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
       <c r="Q6" s="27" t="s">
         <v>4</v>
       </c>
@@ -11018,77 +11050,77 @@
       <c r="J11" s="33"/>
     </row>
     <row r="39" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="51" t="s">
+      <c r="A39" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="B39" s="51"/>
-      <c r="C39" s="51" t="s">
+      <c r="B39" s="53"/>
+      <c r="C39" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="D39" s="51"/>
-      <c r="E39" s="51"/>
-      <c r="F39" s="51"/>
-      <c r="G39" s="51" t="s">
+      <c r="D39" s="53"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="53"/>
+      <c r="G39" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="H39" s="51"/>
-      <c r="I39" s="51"/>
+      <c r="H39" s="53"/>
+      <c r="I39" s="53"/>
       <c r="J39" s="31" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="168.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="49" t="s">
+      <c r="A40" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="B40" s="50"/>
-      <c r="C40" s="52" t="s">
+      <c r="B40" s="52"/>
+      <c r="C40" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="D40" s="52"/>
-      <c r="E40" s="52"/>
-      <c r="F40" s="52"/>
-      <c r="G40" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="H40" s="52"/>
-      <c r="I40" s="52"/>
+      <c r="D40" s="54"/>
+      <c r="E40" s="54"/>
+      <c r="F40" s="54"/>
+      <c r="G40" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="H40" s="54"/>
+      <c r="I40" s="54"/>
       <c r="J40" s="34"/>
     </row>
     <row r="41" spans="1:10" ht="168.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="37" t="s">
+      <c r="A41" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="B41" s="38"/>
-      <c r="C41" s="39" t="s">
+      <c r="B41" s="40"/>
+      <c r="C41" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="39" t="s">
+      <c r="D41" s="41"/>
+      <c r="E41" s="41"/>
+      <c r="F41" s="41"/>
+      <c r="G41" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="H41" s="40"/>
-      <c r="I41" s="40"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="42"/>
       <c r="J41" s="32"/>
     </row>
     <row r="42" spans="1:10" ht="168.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="37" t="s">
+      <c r="A42" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="B42" s="38"/>
-      <c r="C42" s="39" t="s">
+      <c r="B42" s="40"/>
+      <c r="C42" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="D42" s="39"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39" t="s">
+      <c r="D42" s="41"/>
+      <c r="E42" s="41"/>
+      <c r="F42" s="41"/>
+      <c r="G42" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="H42" s="40"/>
-      <c r="I42" s="40"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="42"/>
       <c r="J42" s="32"/>
     </row>
     <row r="43" spans="1:10" ht="168.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -11110,62 +11142,81 @@
       <c r="J43" s="30"/>
     </row>
     <row r="44" spans="1:10" ht="168.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="37" t="s">
+      <c r="A44" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="B44" s="38"/>
-      <c r="C44" s="39" t="s">
+      <c r="B44" s="40"/>
+      <c r="C44" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="D44" s="39"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39" t="s">
+      <c r="D44" s="41"/>
+      <c r="E44" s="41"/>
+      <c r="F44" s="41"/>
+      <c r="G44" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
       <c r="J44" s="32"/>
     </row>
     <row r="45" spans="1:10" ht="168.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="37" t="s">
+      <c r="A45" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="38"/>
-      <c r="C45" s="39" t="s">
+      <c r="B45" s="40"/>
+      <c r="C45" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="D45" s="39"/>
-      <c r="E45" s="39"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="39" t="s">
+      <c r="D45" s="41"/>
+      <c r="E45" s="41"/>
+      <c r="F45" s="41"/>
+      <c r="G45" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="H45" s="40"/>
-      <c r="I45" s="40"/>
+      <c r="H45" s="42"/>
+      <c r="I45" s="42"/>
       <c r="J45" s="32"/>
     </row>
     <row r="46" spans="1:10" ht="168.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="37" t="s">
+      <c r="A46" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="B46" s="38"/>
-      <c r="C46" s="39" t="s">
+      <c r="B46" s="40"/>
+      <c r="C46" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="D46" s="39"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="39"/>
-      <c r="G46" s="39" t="s">
+      <c r="D46" s="41"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="41"/>
+      <c r="G46" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="H46" s="40"/>
-      <c r="I46" s="40"/>
+      <c r="H46" s="42"/>
+      <c r="I46" s="42"/>
       <c r="J46" s="32"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="35">
+    <mergeCell ref="A2:C4"/>
+    <mergeCell ref="H2:J4"/>
+    <mergeCell ref="A5:C6"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="C39:F39"/>
+    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="G39:I39"/>
+    <mergeCell ref="H5:J6"/>
+    <mergeCell ref="D2:G5"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="G43:I43"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:F41"/>
+    <mergeCell ref="G41:I41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:F42"/>
+    <mergeCell ref="G42:I42"/>
     <mergeCell ref="M4:P4"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="K6:L6"/>
@@ -11182,25 +11233,6 @@
     <mergeCell ref="G45:I45"/>
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="C43:F43"/>
-    <mergeCell ref="G43:I43"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:F41"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:F42"/>
-    <mergeCell ref="G42:I42"/>
-    <mergeCell ref="A2:C4"/>
-    <mergeCell ref="H2:J4"/>
-    <mergeCell ref="A5:C6"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C40:F40"/>
-    <mergeCell ref="C39:F39"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="H5:J6"/>
-    <mergeCell ref="D2:G5"/>
-    <mergeCell ref="D6:G6"/>
   </mergeCells>
   <pageMargins left="0.45" right="0.57291666666666663" top="1.1145833333333299" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11218,7 +11250,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:O27"/>
   <sheetViews>
@@ -11579,7 +11611,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:QB1624"/>
   <sheetViews>

</xml_diff>